<commit_message>
new changes to subject ID - added diet_group to 740/764
</commit_message>
<xml_diff>
--- a/norm_correct_avgdsubj_NPI_v1.xlsx
+++ b/norm_correct_avgdsubj_NPI_v1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lplab\Documents\composite_variables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitchtho\Documents\behavior_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -284,7 +284,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -732,15 +732,15 @@
   <dimension ref="A1:AO22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.90625" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -865,7 +865,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -990,7 +990,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>3.5178926698828086</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>2.4039057629080394</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>35740</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -3365,7 +3365,7 @@
         <v>-0.31167360172583408</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>35764</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -3504,9 +3504,9 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>34404</v>
       </c>
@@ -3518,7 +3518,7 @@
       </c>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>34266</v>
       </c>
@@ -3527,7 +3527,7 @@
       </c>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>34477</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>34527</v>
       </c>
@@ -3547,7 +3547,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>34691</v>
       </c>
@@ -3556,7 +3556,7 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>34376</v>
       </c>
@@ -3565,7 +3565,7 @@
       </c>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>34412</v>
       </c>
@@ -3577,7 +3577,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>34680</v>
       </c>
@@ -3586,7 +3586,7 @@
       </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>34352</v>
       </c>
@@ -3595,7 +3595,7 @@
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>34577</v>
       </c>
@@ -3604,7 +3604,7 @@
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>35331</v>
       </c>
@@ -3613,7 +3613,7 @@
       </c>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>35408</v>
       </c>
@@ -3625,7 +3625,7 @@
       </c>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>35435</v>
       </c>
@@ -3634,7 +3634,7 @@
       </c>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>35444</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>35455</v>
       </c>
@@ -3654,7 +3654,7 @@
       </c>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>35476</v>
       </c>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>35505</v>
       </c>
@@ -3672,7 +3672,7 @@
       </c>
       <c r="D17" s="9"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>35600</v>
       </c>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>35624</v>
       </c>
@@ -3690,7 +3690,7 @@
       </c>
       <c r="D19" s="9"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>35712</v>
       </c>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>35716</v>
       </c>
@@ -3708,7 +3708,7 @@
       </c>
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>35375</v>
       </c>
@@ -3717,7 +3717,7 @@
       </c>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>35740</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>35764</v>
       </c>

</xml_diff>